<commit_message>
finalized reporting pages 1 - 3
</commit_message>
<xml_diff>
--- a/Dashboard.xlsx
+++ b/Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonckheerej\Source\Repos\voxmusicawebshopreporting2\VoxMusicaWebshopReporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2271B89E-2085-4BB1-8BA7-DB8AEDE7B479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D766A0-B6FC-4F62-B549-870AB77185E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht Per Klant" sheetId="5" r:id="rId1"/>
@@ -1665,25 +1665,7 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1707,7 +1689,25 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1762,22 +1762,22 @@
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{5CECF9F0-5427-4C7D-A5E7-7B1B761707FA}" uniqueName="1" name="BestelNummer" totalsRowLabel="Total" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{F15B56EE-FA27-4715-A7DF-7CDFEB090CBE}" uniqueName="2" name="BestelDatum" queryTableFieldId="2" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{6F861197-1E83-405C-9E40-E67BA9EAA83A}" uniqueName="3" name="TotaalBedrag" totalsRowFunction="sum" queryTableFieldId="3" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{4D641D52-732D-48EB-933A-D66645F4F14D}" uniqueName="4" name="BetaalMethode" queryTableFieldId="4" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{389CC715-1A18-447D-9C74-07380A9CA069}" uniqueName="5" name="BetalingOK" queryTableFieldId="5" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{F2219184-C52B-4EF7-B8F9-2140D9EF59BF}" uniqueName="18" name="BestelStatus" queryTableFieldId="18" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{F5C6EE80-55EC-4454-9597-30EB9C52B132}" uniqueName="6" name="Voornaam" queryTableFieldId="6" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{6D4E5AB0-CB33-4ACD-86EF-8B4FE87F8684}" uniqueName="7" name="Familienaam" queryTableFieldId="7" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{F90AC6E8-09CD-4C0C-8D43-3B9C169CF368}" uniqueName="8" name="EmailAdres" queryTableFieldId="8" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{92F3221C-36F4-40C6-B420-B999F7E1D875}" uniqueName="9" name="TelefoonNummer" queryTableFieldId="9" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{10C847D4-DB1B-48AA-BC94-726EE827055C}" uniqueName="10" name="Bolognese_0,3l" queryTableFieldId="10"/>
-    <tableColumn id="11" xr3:uid="{6EF0CEA2-DE32-4BEB-B01D-0A10139BB2AA}" uniqueName="11" name="Bolognese_1l" queryTableFieldId="11"/>
+    <tableColumn id="3" xr3:uid="{6F861197-1E83-405C-9E40-E67BA9EAA83A}" uniqueName="3" name="TotaalBedrag" totalsRowFunction="sum" queryTableFieldId="3" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{4D641D52-732D-48EB-933A-D66645F4F14D}" uniqueName="4" name="BetaalMethode" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{389CC715-1A18-447D-9C74-07380A9CA069}" uniqueName="5" name="BetalingOK" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{F2219184-C52B-4EF7-B8F9-2140D9EF59BF}" uniqueName="18" name="BestelStatus" queryTableFieldId="18" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{F5C6EE80-55EC-4454-9597-30EB9C52B132}" uniqueName="6" name="Voornaam" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{6D4E5AB0-CB33-4ACD-86EF-8B4FE87F8684}" uniqueName="7" name="Familienaam" queryTableFieldId="7" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{F90AC6E8-09CD-4C0C-8D43-3B9C169CF368}" uniqueName="8" name="EmailAdres" queryTableFieldId="8" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{92F3221C-36F4-40C6-B420-B999F7E1D875}" uniqueName="9" name="TelefoonNummer" queryTableFieldId="9" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{10C847D4-DB1B-48AA-BC94-726EE827055C}" uniqueName="10" name="Bolognese_0,3l" totalsRowFunction="sum" queryTableFieldId="10"/>
+    <tableColumn id="11" xr3:uid="{6EF0CEA2-DE32-4BEB-B01D-0A10139BB2AA}" uniqueName="11" name="Bolognese_1l" totalsRowFunction="sum" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{7F3457DA-C222-4D90-8206-5E5F6BA4C466}" uniqueName="12" name="Carbonara_0,3l" queryTableFieldId="12"/>
     <tableColumn id="13" xr3:uid="{E77BFD8A-48A2-477E-A602-75067636DA74}" uniqueName="13" name="Carbonara_1l" queryTableFieldId="13"/>
     <tableColumn id="14" xr3:uid="{D69CBE67-FBDB-4219-ACB2-3419459EB538}" uniqueName="14" name="Veggie_0,3l" queryTableFieldId="14"/>
     <tableColumn id="15" xr3:uid="{DD595D7D-620A-4AAB-8A5D-06A5B7FCA78D}" uniqueName="15" name="Veggie_1l" queryTableFieldId="15"/>
     <tableColumn id="16" xr3:uid="{A89EEF17-0E8B-4B08-B122-739A60BF5327}" uniqueName="16" name="GratisSoubryPasta" queryTableFieldId="16"/>
-    <tableColumn id="17" xr3:uid="{168A0DE1-2C44-4EEF-B3DD-76EA7AFA8DBC}" uniqueName="17" name="Volledige naam" totalsRowFunction="count" queryTableFieldId="17" dataDxfId="2">
+    <tableColumn id="17" xr3:uid="{168A0DE1-2C44-4EEF-B3DD-76EA7AFA8DBC}" uniqueName="17" name="Volledige naam" totalsRowFunction="count" queryTableFieldId="17" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT(SpaghettiActieOverzicht2024[[#This Row],[Voornaam]]," ",SpaghettiActieOverzicht2024[[#This Row],[Familienaam]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="19" xr3:uid="{795EBA2E-0790-4F95-A5ED-39BA76BF85DE}" uniqueName="19" name="Opgehaald" queryTableFieldId="20"/>
@@ -2052,7 +2052,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2632,8 +2632,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:S95"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="55" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M95" sqref="M95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8306,6 +8306,14 @@
         <f>SUBTOTAL(109,SpaghettiActieOverzicht2024[TotaalBedrag])</f>
         <v>0</v>
       </c>
+      <c r="K95">
+        <f>SUBTOTAL(109,SpaghettiActieOverzicht2024[Bolognese_0,3l])</f>
+        <v>15</v>
+      </c>
+      <c r="L95">
+        <f>SUBTOTAL(109,SpaghettiActieOverzicht2024[Bolognese_1l])</f>
+        <v>123</v>
+      </c>
       <c r="R95">
         <f>SUBTOTAL(103,SpaghettiActieOverzicht2024[Volledige naam])</f>
         <v>93</v>

</xml_diff>